<commit_message>
fixed plc parsing logic and wayside mapping in the excel
</commit_message>
<xml_diff>
--- a/src/main/TrackController/greenLine.xlsx
+++ b/src/main/TrackController/greenLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiqu\Desktop\ECE1140\ECE-1140\src\main\TrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E095C36D-A154-41EC-8D42-E5106436BB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0C78D-A13B-4255-8D08-D9B736980B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="55">
   <si>
     <t>Block Number</t>
   </si>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCA0872-F3C1-4B8E-B7BD-13508CAEC5E4}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,9 +1123,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1G</v>
+      <c r="A33" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B33" s="2">
         <v>30</v>
@@ -1143,7 +1142,7 @@
     <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B34" s="2">
         <v>30</v>
@@ -1159,7 +1158,7 @@
     <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B35" s="2">
         <v>30</v>
@@ -1175,7 +1174,7 @@
     <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B36" s="2">
         <v>30</v>
@@ -1191,7 +1190,7 @@
     <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B37" s="2">
         <v>30</v>
@@ -1207,7 +1206,7 @@
     <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B38" s="2">
         <v>30</v>
@@ -1225,7 +1224,7 @@
     <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="str">
         <f>A35</f>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B39" s="2">
         <v>30</v>
@@ -1243,7 +1242,7 @@
     <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B40" s="2">
         <v>30</v>
@@ -1261,7 +1260,7 @@
     <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B41" s="2">
         <v>30</v>
@@ -1279,7 +1278,7 @@
     <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B42" s="2">
         <v>30</v>
@@ -1297,7 +1296,7 @@
     <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B43" s="2">
         <v>30</v>
@@ -1315,7 +1314,7 @@
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B44" s="2">
         <v>30</v>
@@ -1333,7 +1332,7 @@
     <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B45" s="2">
         <v>30</v>
@@ -1351,7 +1350,7 @@
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B46" s="2">
         <v>30</v>
@@ -1369,7 +1368,7 @@
     <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B47" s="2">
         <v>30</v>
@@ -1387,7 +1386,7 @@
     <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B48" s="2">
         <v>30</v>
@@ -1405,7 +1404,7 @@
     <row r="49" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B49" s="2">
         <v>30</v>
@@ -1423,7 +1422,7 @@
     <row r="50" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B50" s="2">
         <v>30</v>
@@ -1441,7 +1440,7 @@
     <row r="51" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B51" s="2">
         <v>30</v>
@@ -1459,7 +1458,7 @@
     <row r="52" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B52" s="2">
         <v>30</v>
@@ -1477,7 +1476,7 @@
     <row r="53" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B53" s="2">
         <v>30</v>
@@ -1495,7 +1494,7 @@
     <row r="54" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B54" s="2">
         <v>30</v>
@@ -1513,7 +1512,7 @@
     <row r="55" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B55" s="2">
         <v>30</v>
@@ -1531,7 +1530,7 @@
     <row r="56" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B56" s="2">
         <v>30</v>
@@ -1549,7 +1548,7 @@
     <row r="57" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B57" s="2">
         <v>30</v>
@@ -1567,7 +1566,7 @@
     <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B58" s="2">
         <v>30</v>
@@ -1585,7 +1584,7 @@
     <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B59" s="2">
         <v>30</v>
@@ -1603,7 +1602,7 @@
     <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>wayside1G</v>
+        <v>wayside2G</v>
       </c>
       <c r="B60" s="2">
         <v>30</v>

</xml_diff>

<commit_message>
I don't even know whats happening at this point
</commit_message>
<xml_diff>
--- a/src/main/TrackController/greenLine.xlsx
+++ b/src/main/TrackController/greenLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiqu\Desktop\ECE1140\ECE-1140\src\main\TrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0C78D-A13B-4255-8D08-D9B736980B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4809A7-E3BD-4FCB-B767-B770BAF3B927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCA0872-F3C1-4B8E-B7BD-13508CAEC5E4}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +799,9 @@
       <c r="C13" s="2">
         <v>11</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>4</v>
       </c>
@@ -832,9 +834,6 @@
       </c>
       <c r="C15" s="2">
         <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
I don't remmeber my changes
</commit_message>
<xml_diff>
--- a/src/main/TrackController/greenLine.xlsx
+++ b/src/main/TrackController/greenLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiqu\Desktop\ECE1140\ECE-1140\src\main\TrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768983F6-E383-4EB5-97D2-FB24A4EB5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C493F444-1767-41D8-B9F3-1742F7DD2ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,7 +578,7 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
integration with track model for lights and crossing
</commit_message>
<xml_diff>
--- a/src/main/TrackController/greenLine.xlsx
+++ b/src/main/TrackController/greenLine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiqu\Desktop\ECE1140\ECE-1140\src\main\TrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D5BF61-C75E-42CA-84A2-FC6FE403E7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9AB9CA-B501-4E3B-BEBC-4F981AD228DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green_info" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="56">
   <si>
     <t>Block Number</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>junctionWS;0;62;0;green</t>
+  </si>
+  <si>
+    <t>junctionNS;green</t>
   </si>
 </sst>
 </file>
@@ -577,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCA0872-F3C1-4B8E-B7BD-13508CAEC5E4}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>51</v>
@@ -634,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
@@ -814,9 +817,7 @@
       <c r="C14" s="4">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1114,9 +1115,7 @@
       <c r="C32" s="4">
         <v>30</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
@@ -1670,9 +1669,7 @@
       <c r="C64" s="4">
         <v>62</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>12</v>
       </c>
@@ -1889,7 +1886,7 @@
         <v>76</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>15</v>
@@ -2044,9 +2041,7 @@
       <c r="C88" s="4">
         <v>86</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D88" s="2"/>
       <c r="E88" s="2" t="s">
         <v>17</v>
       </c>
@@ -2261,7 +2256,7 @@
         <v>100</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>19</v>
@@ -2277,9 +2272,7 @@
       <c r="C103" s="2">
         <v>101</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D103" s="2"/>
       <c r="E103" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3057,7 @@
         <v>150</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>29</v>

</xml_diff>